<commit_message>
adding validation to program
</commit_message>
<xml_diff>
--- a/process_inputs.xlsx
+++ b/process_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willy\Developer\Labaton\LabatonSlipMerge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC882667-7A55-4FC5-BA77-F72E22C34E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0175239A-9EEB-4097-A42A-A95C8D88D434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5475" yWindow="1845" windowWidth="26085" windowHeight="16290" xr2:uid="{ECE956F9-C328-4E55-B74B-D0ECF1A979DB}"/>
+    <workbookView xWindow="5820" yWindow="2190" windowWidth="26085" windowHeight="16290" activeTab="1" xr2:uid="{ECE956F9-C328-4E55-B74B-D0ECF1A979DB}"/>
   </bookViews>
   <sheets>
     <sheet name="FileList" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
   <si>
     <t>Treatment Type</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Input File</t>
+  </si>
+  <si>
+    <t>Input/GenericSlip</t>
   </si>
 </sst>
 </file>
@@ -464,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68987694-470D-4C6D-9411-E970925FEB84}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +550,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -562,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428216A2-907F-49E5-BDA2-4C920EA87DCE}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +603,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>

</xml_diff>